<commit_message>
Exercicio 3 feito - Talvez falte views
</commit_message>
<xml_diff>
--- a/Task 3.xlsx
+++ b/Task 3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guicu\Documents\Universidade\Mestrado\2º Semestre\Aplicações na web\aw-project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafae\OneDrive\Ambiente de Trabalho\MESTRADO\2 semestre\Aplicações em Web\aw-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F774A158-35BE-4201-81E9-CCF5EC97F354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D40F649-D66E-4727-9D1A-32CADC0A580F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DF0E2589-CB8B-477F-AEE2-76A16165ADDE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DF0E2589-CB8B-477F-AEE2-76A16165ADDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
   <si>
     <t>Views</t>
   </si>
@@ -55,6 +55,93 @@
   </si>
   <si>
     <t>Account</t>
+  </si>
+  <si>
+    <t>Stats</t>
+  </si>
+  <si>
+    <t>Move Positive</t>
+  </si>
+  <si>
+    <t>Move Negative</t>
+  </si>
+  <si>
+    <t>Saved Products</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Map </t>
+  </si>
+  <si>
+    <t>Categories</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Market</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>Talvez tenha?</t>
+  </si>
+  <si>
+    <t>Highlights</t>
+  </si>
+  <si>
+    <t>Meat</t>
+  </si>
+  <si>
+    <t>Expand</t>
+  </si>
+  <si>
+    <t>Feedback</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Market </t>
+  </si>
+  <si>
+    <t>All products</t>
+  </si>
+  <si>
+    <t>Info</t>
+  </si>
+  <si>
+    <t>Qrcode</t>
+  </si>
+  <si>
+    <t>Meat Scanned</t>
+  </si>
+  <si>
+    <t>See more</t>
+  </si>
+  <si>
+    <t>Não é suposto fazer me thinks</t>
+  </si>
+  <si>
+    <t>Meat?</t>
+  </si>
+  <si>
+    <t>Year bar</t>
+  </si>
+  <si>
+    <t>Top graphs</t>
+  </si>
+  <si>
+    <t>Bottom graphs</t>
+  </si>
+  <si>
+    <t>Meat photo</t>
+  </si>
+  <si>
+    <t>Meat details</t>
+  </si>
+  <si>
+    <t>Header</t>
+  </si>
+  <si>
+    <t>Slider</t>
   </si>
 </sst>
 </file>
@@ -156,21 +243,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -180,6 +259,27 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -251,16 +351,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>79093</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>320706</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>513844</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>78027</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>167356</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>26979</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1344706</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>384036</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -289,8 +389,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13924633" y="2385726"/>
-          <a:ext cx="697863" cy="1413153"/>
+          <a:off x="8638109" y="750380"/>
+          <a:ext cx="830862" cy="1695538"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -301,16 +401,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>84313</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>210575</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>512802</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>139134</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>172576</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>252127</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1352085</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>90156</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -339,8 +439,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13929853" y="881135"/>
-          <a:ext cx="697863" cy="1413152"/>
+          <a:off x="8648546" y="2634219"/>
+          <a:ext cx="839283" cy="1651583"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -400,23 +500,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>197930</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>439892</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>364187</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>159457</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>286193</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>38397</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1159017</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>348156</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Imagem 14">
+        <xdr:cNvPr id="19" name="Imagem 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3E099C8-3878-D2E9-DA3C-FAB5163447F6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F716A0CA-8F03-F680-3719-40BFCEDB4291}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -424,7 +524,7 @@
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill>
+      <xdr:blipFill rotWithShape="1">
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
@@ -432,14 +532,13 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:srcRect b="15452"/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7947470" y="2504912"/>
-          <a:ext cx="697863" cy="1404445"/>
+          <a:off x="2525377" y="8429785"/>
+          <a:ext cx="794830" cy="1357974"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -450,23 +549,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>528410</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>14941</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>338163</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>367997</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>7073</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>64115</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1234109</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>330121</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="19" name="Imagem 18">
+        <xdr:cNvPr id="21" name="Imagem 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F716A0CA-8F03-F680-3719-40BFCEDB4291}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4DE866A-7128-9D6C-B2AC-CA5FA7C2CA60}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -474,7 +573,7 @@
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill>
+      <xdr:blipFill rotWithShape="1">
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
@@ -482,14 +581,13 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:srcRect b="18475"/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8887550" y="2537161"/>
-          <a:ext cx="697863" cy="1413154"/>
+          <a:off x="2499924" y="10381671"/>
+          <a:ext cx="895946" cy="1469559"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -500,23 +598,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>80546</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>430590</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>279772</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>223501</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>168809</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>45422</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1225825</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>39421</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="Imagem 20">
+        <xdr:cNvPr id="23" name="Imagem 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4DE866A-7128-9D6C-B2AC-CA5FA7C2CA60}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CBA9759-19DF-0FD2-F621-77A4F1FA4B1E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -524,7 +622,7 @@
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill>
+      <xdr:blipFill rotWithShape="1">
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
@@ -532,14 +630,13 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:srcRect b="16686"/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9658886" y="2495610"/>
-          <a:ext cx="697863" cy="1413152"/>
+          <a:off x="2441533" y="12581153"/>
+          <a:ext cx="946053" cy="1580116"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -550,23 +647,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>245786</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>46139</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>331010</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>135422</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>334049</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>87692</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1196995</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>751588</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="23" name="Imagem 22">
+        <xdr:cNvPr id="27" name="Imagem 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CBA9759-19DF-0FD2-F621-77A4F1FA4B1E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83B27889-D50D-B3D5-3D25-7332A2BC72F3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -574,7 +671,7 @@
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill>
+      <xdr:blipFill rotWithShape="1">
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
@@ -582,14 +679,13 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:srcRect b="17209"/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9824126" y="716699"/>
-          <a:ext cx="697863" cy="1413153"/>
+          <a:off x="2492452" y="15316807"/>
+          <a:ext cx="865985" cy="1447193"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -600,23 +696,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>251006</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>149368</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>366427</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>156620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>339269</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>182212</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1123293</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>212428</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="25" name="Imagem 24">
+        <xdr:cNvPr id="31" name="Imagem 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8AE936E-47E2-62B6-9E83-C22910AF757B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE1F8664-2D4F-5A32-8A34-742623342B9E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -624,7 +720,7 @@
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill>
+      <xdr:blipFill rotWithShape="1">
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
@@ -632,14 +728,13 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:srcRect b="17246"/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12877346" y="819928"/>
-          <a:ext cx="697863" cy="1404444"/>
+          <a:off x="2527617" y="6791275"/>
+          <a:ext cx="756866" cy="1264498"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -650,23 +745,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>256226</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>414758</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>367863</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>140292</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>344489</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>41870</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1128631</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>154768</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="27" name="Imagem 26">
+        <xdr:cNvPr id="33" name="Imagem 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83B27889-D50D-B3D5-3D25-7332A2BC72F3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9241916E-320C-1CEA-B1FB-8D314EC20B9B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -674,7 +769,7 @@
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill>
+      <xdr:blipFill rotWithShape="1">
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
@@ -682,14 +777,13 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:srcRect b="17582"/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10444166" y="2479778"/>
-          <a:ext cx="697863" cy="1402572"/>
+          <a:off x="2529053" y="5145844"/>
+          <a:ext cx="760768" cy="1262579"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -700,23 +794,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>387483</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>36837</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>424686</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>113158</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>475746</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>78390</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1122549</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>104178</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="29" name="Imagem 28">
+        <xdr:cNvPr id="35" name="Imagem 34">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5D407A5-B3EA-110E-2A14-3ACEEF23158A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1388CE95-8672-C118-DA7F-891E04BEA808}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -724,7 +818,7 @@
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill>
+      <xdr:blipFill rotWithShape="1">
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
@@ -732,14 +826,13 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:srcRect b="17391"/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10575423" y="707397"/>
-          <a:ext cx="697863" cy="1413153"/>
+          <a:off x="2585129" y="3511851"/>
+          <a:ext cx="697863" cy="1168657"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -750,123 +843,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>583203</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>307706</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>288960</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>362777</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>61866</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>13980</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1226870</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>149086</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="31" name="Imagem 30">
+        <xdr:cNvPr id="37" name="Imagem 36">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE1F8664-2D4F-5A32-8A34-742623342B9E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11380743" y="2372726"/>
-          <a:ext cx="697863" cy="1413154"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>55023</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>258535</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>143286</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>300088</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="33" name="Imagem 32">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9241916E-320C-1CEA-B1FB-8D314EC20B9B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11462163" y="929095"/>
-          <a:ext cx="697863" cy="1413153"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>422955</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>367860</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1120818</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>76841</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="35" name="Imagem 34">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1388CE95-8672-C118-DA7F-891E04BEA808}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A01B941-02A6-98E0-295F-51049610827E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -875,70 +868,20 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect b="17391"/>
+        <a:srcRect b="17039"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2648123" y="3323011"/>
-          <a:ext cx="697863" cy="1152939"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>138160</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>152572</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>226423</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>185417</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="37" name="Imagem 36">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A01B941-02A6-98E0-295F-51049610827E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12154900" y="823132"/>
-          <a:ext cx="697863" cy="1404445"/>
+          <a:off x="2450721" y="15072690"/>
+          <a:ext cx="937910" cy="1550505"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -951,9 +894,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -991,7 +934,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1097,7 +1040,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1239,7 +1182,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1247,22 +1190,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{832E6391-5178-4AA5-93E0-67A87F0C74F9}">
-  <dimension ref="B1:D10"/>
+  <dimension ref="B1:H38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B7" zoomScale="252" zoomScaleNormal="35" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.44140625" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" customWidth="1"/>
-    <col min="4" max="4" width="31.5546875" customWidth="1"/>
+    <col min="1" max="1" width="32.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" customWidth="1"/>
+    <col min="4" max="4" width="31.42578125" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" customWidth="1"/>
+    <col min="7" max="8" width="31.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:4" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:8" ht="31.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1272,69 +1218,364 @@
       <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="3"/>
-      <c r="C3" s="4" t="s">
+      <c r="F2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="2"/>
+      <c r="C3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="3"/>
-      <c r="C4" s="4" t="s">
+      <c r="D3" s="10"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+      <c r="C4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="3"/>
-      <c r="C5" s="4" t="s">
+      <c r="D4" s="10"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="2"/>
+      <c r="C5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="3"/>
-      <c r="C6" s="5" t="s">
+      <c r="D5" s="10"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+    </row>
+    <row r="6" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="2"/>
+      <c r="C6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="7"/>
-      <c r="C7" s="4" t="s">
+      <c r="D6" s="10"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="3"/>
+      <c r="C7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="8"/>
-      <c r="C8" s="4" t="s">
+      <c r="D7" s="10"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+    </row>
+    <row r="8" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
+      <c r="C8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="9"/>
-      <c r="C9" s="4" t="s">
+      <c r="F8" s="3"/>
+      <c r="G8" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="2:8" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="5"/>
+      <c r="C9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="6"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="2"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="3"/>
+      <c r="C10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="2:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="C11" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+      <c r="C12" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+    </row>
+    <row r="13" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="5"/>
+      <c r="C13" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="3"/>
+      <c r="C14" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="10"/>
+    </row>
+    <row r="15" spans="2:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+      <c r="C15" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
+      <c r="C16" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="5"/>
+      <c r="C17" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="3"/>
+      <c r="C18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+    </row>
+    <row r="20" spans="2:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="4"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+    </row>
+    <row r="22" spans="2:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="3"/>
+      <c r="C22" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="4"/>
+      <c r="C23" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
+      <c r="C24" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="3"/>
+      <c r="C25" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="9"/>
+    </row>
+    <row r="26" spans="2:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="4"/>
+      <c r="C26" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="9"/>
+    </row>
+    <row r="27" spans="2:4" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="4"/>
+      <c r="C27" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="3"/>
+      <c r="C28" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="4"/>
+      <c r="C29" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="4"/>
+      <c r="C30" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="4"/>
+      <c r="C31" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="3"/>
+      <c r="C32" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="4"/>
+      <c r="C33" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33" s="9"/>
+    </row>
+    <row r="34" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="4"/>
+      <c r="C34" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="4"/>
+      <c r="C35" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="65.849999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="3"/>
+      <c r="C36" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D36" s="9"/>
+    </row>
+    <row r="37" spans="2:4" ht="65.849999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="5"/>
+      <c r="C37" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="12"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="20">
+    <mergeCell ref="G8:G12"/>
+    <mergeCell ref="H8:H12"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H3:H5"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="F3:F7"/>
+    <mergeCell ref="F8:F12"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="D18:D21"/>
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>